<commit_message>
Added Naive Component Forecasting
</commit_message>
<xml_diff>
--- a/0_0_Data/3_Naive_Forecaster_Data/0_Combined_QoQ_Forecasts/dt_full_CONSTR_qoqAVERAGE_10_9.xlsx
+++ b/0_0_Data/3_Naive_Forecaster_Data/0_Combined_QoQ_Forecasts/dt_full_CONSTR_qoqAVERAGE_10_9.xlsx
@@ -1342,6 +1342,9 @@
       <c r="A7" s="1">
         <v>39994</v>
       </c>
+      <c r="B7">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C7">
         <v>0.7444112022064786</v>
       </c>
@@ -1500,6 +1503,9 @@
       <c r="A8" s="1">
         <v>40086</v>
       </c>
+      <c r="B8">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C8">
         <v>0.8555642925598477</v>
       </c>
@@ -1658,6 +1664,9 @@
       <c r="A9" s="1">
         <v>40178</v>
       </c>
+      <c r="B9">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C9">
         <v>0.7667663204885145</v>
       </c>
@@ -1816,6 +1825,9 @@
       <c r="A10" s="1">
         <v>40268</v>
       </c>
+      <c r="B10">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C10">
         <v>0.7226490915834205</v>
       </c>
@@ -1974,11 +1986,14 @@
       <c r="A11" s="1">
         <v>40359</v>
       </c>
+      <c r="B11">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C11">
-        <v>-0.03000204061924873</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D11">
-        <v>-1.220171743119447</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E11">
         <v>-0.02547741087713007</v>
@@ -2132,11 +2147,14 @@
       <c r="A12" s="1">
         <v>40451</v>
       </c>
+      <c r="B12">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C12">
-        <v>0.02438177501188936</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D12">
-        <v>-0.5867161878436726</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E12">
         <v>0.4311871488147432</v>
@@ -2290,11 +2308,14 @@
       <c r="A13" s="1">
         <v>40543</v>
       </c>
+      <c r="B13">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C13">
-        <v>-0.06535641406540374</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D13">
-        <v>-0.6347479511340203</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E13">
         <v>0.5190127646174574</v>
@@ -2448,11 +2469,14 @@
       <c r="A14" s="1">
         <v>40633</v>
       </c>
+      <c r="B14">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C14">
-        <v>-0.05210103033034684</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D14">
-        <v>-0.727215211743783</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E14">
         <v>0.5196249850277752</v>
@@ -2606,17 +2630,20 @@
       <c r="A15" s="1">
         <v>40724</v>
       </c>
+      <c r="B15">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C15">
-        <v>-0.06333478985005078</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D15">
-        <v>-0.6745623117652879</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E15">
-        <v>-0.2719696311759744</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F15">
-        <v>-0.4065793976801036</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G15">
         <v>-0.1965369824803531</v>
@@ -2764,17 +2791,20 @@
       <c r="A16" s="1">
         <v>40816</v>
       </c>
+      <c r="B16">
+        <v>0.4789635212487423</v>
+      </c>
       <c r="C16">
-        <v>-0.06094347173711489</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D16">
-        <v>-0.6827394491906246</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E16">
-        <v>-0.1091309750828</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F16">
-        <v>-0.2877553014448807</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G16">
         <v>-0.7922079768977568</v>
@@ -2923,16 +2953,16 @@
         <v>40908</v>
       </c>
       <c r="C17">
-        <v>-0.06240751502655286</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D17">
-        <v>-0.6884380410757039</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E17">
-        <v>-0.1766195723728647</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F17">
-        <v>-0.3296460258199556</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G17">
         <v>-1.062265519602065</v>
@@ -3081,16 +3111,16 @@
         <v>40999</v>
       </c>
       <c r="C18">
-        <v>-0.06202050539436126</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D18">
-        <v>-0.6842437349129307</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E18">
-        <v>-0.1557453450331039</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F18">
-        <v>-0.3159735784669054</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G18">
         <v>-0.911621726278625</v>
@@ -3239,22 +3269,22 @@
         <v>41090</v>
       </c>
       <c r="C19">
-        <v>-0.06221725405092401</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D19">
-        <v>-0.6851985412057341</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E19">
-        <v>-0.162937106768641</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F19">
-        <v>-0.3205143670590444</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G19">
-        <v>-0.1740931065973966</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H19">
-        <v>0.2744621615955504</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I19">
         <v>1.304682315704213</v>
@@ -3397,22 +3427,22 @@
         <v>41182</v>
       </c>
       <c r="C20">
-        <v>-0.0621577921521779</v>
+        <v>-0.07767737160209423</v>
       </c>
       <c r="D20">
-        <v>-0.6855083969387989</v>
+        <v>-0.5592545128004203</v>
       </c>
       <c r="E20">
-        <v>-0.1605614477939769</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F20">
-        <v>-0.3190123619336877</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G20">
-        <v>-0.1319916205157314</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H20">
-        <v>0.282913763829351</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I20">
         <v>1.147881733759064</v>
@@ -3555,16 +3585,16 @@
         <v>41274</v>
       </c>
       <c r="E21">
-        <v>-0.161358928632659</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F21">
-        <v>-0.3195096549784303</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G21">
-        <v>-0.020928220862166</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H21">
-        <v>0.2647707942600089</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I21">
         <v>0.7581248089406643</v>
@@ -3707,16 +3737,16 @@
         <v>41364</v>
       </c>
       <c r="E22">
-        <v>-0.1610928784620075</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F22">
-        <v>-0.3193450431023057</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G22">
-        <v>-0.01169387475810063</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H22">
-        <v>0.2661524433078941</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I22">
         <v>0.6418510343227553</v>
@@ -3859,22 +3889,22 @@
         <v>41455</v>
       </c>
       <c r="E23">
-        <v>-0.1611818480311643</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F23">
-        <v>-0.3193995349007979</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G23">
-        <v>0.005108102362201786</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H23">
-        <v>0.2650042713293362</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I23">
-        <v>0.2491341277874939</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J23">
-        <v>0.2183190198072953</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K23">
         <v>0.472882426562407</v>
@@ -4011,22 +4041,22 @@
         <v>41547</v>
       </c>
       <c r="E24">
-        <v>-0.1611521230610529</v>
+        <v>0.2712053048682151</v>
       </c>
       <c r="F24">
-        <v>-0.319381496574243</v>
+        <v>0.09034521845478594</v>
       </c>
       <c r="G24">
-        <v>0.006932197142995159</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H24">
-        <v>0.2651421770329878</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I24">
-        <v>0.243639787105311</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J24">
-        <v>0.2288410476809929</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K24">
         <v>0.5424560602610171</v>
@@ -4163,16 +4193,16 @@
         <v>41639</v>
       </c>
       <c r="G25">
-        <v>0.009485422992910414</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H25">
-        <v>0.2650670731736547</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I25">
-        <v>0.2286895631380773</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J25">
-        <v>0.2084563903658811</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K25">
         <v>0.5656255759392366</v>
@@ -4309,16 +4339,16 @@
         <v>41729</v>
       </c>
       <c r="G26">
-        <v>0.009825346695294244</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H26">
-        <v>0.2650789265706369</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I26">
-        <v>0.2284397860815932</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J26">
-        <v>0.2089566122473051</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K26">
         <v>0.5657163696486549</v>
@@ -4455,22 +4485,22 @@
         <v>41820</v>
       </c>
       <c r="G27">
-        <v>0.01021500554085203</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H27">
-        <v>0.2650738768242577</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I27">
-        <v>0.2278705395131385</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J27">
-        <v>0.2084414345629045</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K27">
-        <v>0.4261703097446162</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L27">
-        <v>0.4332713120545441</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M27">
         <v>0.3891881756981519</v>
@@ -4601,22 +4631,22 @@
         <v>41912</v>
       </c>
       <c r="G28">
-        <v>0.01027605652108545</v>
+        <v>0.3178976984730341</v>
       </c>
       <c r="H28">
-        <v>0.2650748276390178</v>
+        <v>0.650566118073003</v>
       </c>
       <c r="I28">
-        <v>0.2278594859268122</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J28">
-        <v>0.2084599310816207</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K28">
-        <v>0.41657485246156</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L28">
-        <v>0.4243518165146791</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M28">
         <v>0.5711818380382852</v>
@@ -4747,16 +4777,16 @@
         <v>42004</v>
       </c>
       <c r="I29">
-        <v>0.2278378070107994</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J29">
-        <v>0.208446842936269</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K29">
-        <v>0.4073745498514295</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L29">
-        <v>0.4153210929005642</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M29">
         <v>0.6286173499290442</v>
@@ -4887,16 +4917,16 @@
         <v>42094</v>
       </c>
       <c r="I30">
-        <v>0.2278373274388295</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J30">
-        <v>0.2084474574761183</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K30">
-        <v>0.4061543178160629</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L30">
-        <v>0.4140780956087748</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M30">
         <v>0.6288359190683224</v>
@@ -5027,22 +5057,22 @@
         <v>42185</v>
       </c>
       <c r="I31">
-        <v>0.2278365016692332</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J31">
-        <v>0.2084471232866128</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K31">
-        <v>0.4055073118206693</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L31">
-        <v>0.4133836967595417</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M31">
-        <v>0.6594832956274514</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N31">
-        <v>0.6779311981478835</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O31">
         <v>0.8862767946391017</v>
@@ -5167,22 +5197,22 @@
         <v>42277</v>
       </c>
       <c r="I32">
-        <v>0.2278364811759447</v>
+        <v>0.3540094884652206</v>
       </c>
       <c r="J32">
-        <v>0.208447142532651</v>
+        <v>0.3178689890031748</v>
       </c>
       <c r="K32">
-        <v>0.4053881193515568</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L32">
-        <v>0.4132507536439852</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M32">
-        <v>0.6644280027814712</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N32">
-        <v>0.671325903587542</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O32">
         <v>0.9167686939480291</v>
@@ -5307,16 +5337,16 @@
         <v>42369</v>
       </c>
       <c r="K33">
-        <v>0.4053403223998316</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L33">
-        <v>0.4131946913194416</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M33">
-        <v>0.6670213133751617</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N33">
-        <v>0.6680226658450114</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O33">
         <v>0.9600127617940331</v>
@@ -5441,16 +5471,16 @@
         <v>42460</v>
       </c>
       <c r="K34">
-        <v>0.405329739392459</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L34">
-        <v>0.4131817725205327</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M34">
-        <v>0.6677286650520322</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N34">
-        <v>0.667199938224328</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O34">
         <v>0.9600671730357675</v>
@@ -5575,22 +5605,22 @@
         <v>42551</v>
       </c>
       <c r="K35">
-        <v>0.4053260861239772</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L35">
-        <v>0.4131770902680577</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M35">
-        <v>0.6679946026198631</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N35">
-        <v>0.6669097667126367</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O35">
-        <v>0.6609964603812228</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P35">
-        <v>0.6296168067735319</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q35">
         <v>0.337517971417995</v>
@@ -5709,22 +5739,22 @@
         <v>42643</v>
       </c>
       <c r="K36">
-        <v>0.4053251871002698</v>
+        <v>0.9947567147905432</v>
       </c>
       <c r="L36">
-        <v>0.4131758895458355</v>
+        <v>1.0121950006234</v>
       </c>
       <c r="M36">
-        <v>0.6680788872447362</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N36">
-        <v>0.6668250259683544</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O36">
-        <v>0.6203147707141639</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P36">
-        <v>0.5946995411728259</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q36">
         <v>0.5064407828060808</v>
@@ -5843,16 +5873,16 @@
         <v>42735</v>
       </c>
       <c r="M37">
-        <v>0.6681080489273659</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N37">
-        <v>0.6667977124851148</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O37">
-        <v>0.5994686586342113</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P37">
-        <v>0.5704321679613585</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q37">
         <v>0.6175810576904581</v>
@@ -5971,16 +6001,16 @@
         <v>42825</v>
       </c>
       <c r="M38">
-        <v>0.6681176853592872</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N38">
-        <v>0.666789360664616</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O38">
-        <v>0.594549995377881</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P38">
-        <v>0.5649176775617645</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q38">
         <v>0.6208163030755998</v>
@@ -6099,19 +6129,19 @@
         <v>42916</v>
       </c>
       <c r="M39">
-        <v>0.6681209465374304</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N39">
-        <v>0.6667867347969921</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O39">
-        <v>0.592813592172755</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P39">
-        <v>0.5625760893927632</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q39">
-        <v>0.5167354494528774</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R39">
         <v>0.6273934612667631</v>
@@ -6227,19 +6257,19 @@
         <v>43008</v>
       </c>
       <c r="M40">
-        <v>0.6681220365530709</v>
+        <v>1.366378886353468</v>
       </c>
       <c r="N40">
-        <v>0.6667859213273677</v>
+        <v>1.360777235569103</v>
       </c>
       <c r="O40">
-        <v>0.5923255508788439</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P40">
-        <v>0.5619010197410006</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q40">
-        <v>0.5033682710584223</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R40">
         <v>0.628129929716664</v>
@@ -6355,13 +6385,13 @@
         <v>43100</v>
       </c>
       <c r="O41">
-        <v>0.5921702585746463</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P41">
-        <v>0.5616562982800857</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q41">
-        <v>0.4945274717084783</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R41">
         <v>0.6674945835057713</v>
@@ -6477,13 +6507,13 @@
         <v>43190</v>
       </c>
       <c r="O42">
-        <v>0.5921241462769347</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P42">
-        <v>0.5615791653795383</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q42">
-        <v>0.4924619986707973</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R42">
         <v>0.6678010111104555</v>
@@ -6599,19 +6629,19 @@
         <v>43281</v>
       </c>
       <c r="O43">
-        <v>0.5921099226214085</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P43">
-        <v>0.5615527249514496</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q43">
-        <v>0.4915896296246571</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R43">
-        <v>0.5631811875984641</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S43">
-        <v>0.569354083764499</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T43">
         <v>0.6448074495218208</v>
@@ -6721,19 +6751,19 @@
         <v>43373</v>
       </c>
       <c r="O44">
-        <v>0.5921056268145495</v>
+        <v>0.6836469502297249</v>
       </c>
       <c r="P44">
-        <v>0.5615441116222006</v>
+        <v>0.5865790622172199</v>
       </c>
       <c r="Q44">
-        <v>0.4913349282634432</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R44">
-        <v>0.5496768485677495</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S44">
-        <v>0.5423501598369613</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T44">
         <v>0.6451379409190565</v>
@@ -6843,13 +6873,13 @@
         <v>43465</v>
       </c>
       <c r="Q45">
-        <v>0.4912422032434184</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R45">
-        <v>0.540947377636724</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S45">
-        <v>0.5260161759384705</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T45">
         <v>0.6571457042417137</v>
@@ -6959,13 +6989,13 @@
         <v>43555</v>
       </c>
       <c r="Q46">
-        <v>0.4912127337299375</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R46">
-        <v>0.5389174143649721</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S46">
-        <v>0.5223040101624986</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T46">
         <v>0.6575286109465424</v>
@@ -7075,19 +7105,19 @@
         <v>43646</v>
       </c>
       <c r="Q47">
-        <v>0.4912025649572918</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R47">
-        <v>0.5380722710477135</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S47">
-        <v>0.5208418426970087</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T47">
-        <v>0.5654574044350866</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U47">
-        <v>0.5772555503093409</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V47">
         <v>0.6057317098380395</v>
@@ -7191,19 +7221,19 @@
         <v>43738</v>
       </c>
       <c r="Q48">
-        <v>0.4911992283402341</v>
+        <v>0.3760732847431754</v>
       </c>
       <c r="R48">
-        <v>0.5378275084352283</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S48">
-        <v>0.5204309984719087</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T48">
-        <v>0.5535947378115422</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U48">
-        <v>0.5647984058377991</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V48">
         <v>0.5881173499186332</v>
@@ -7307,16 +7337,16 @@
         <v>43830</v>
       </c>
       <c r="R49">
-        <v>0.5377394507264397</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S49">
-        <v>0.5202901360027036</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T49">
-        <v>0.5470729522729348</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U49">
-        <v>0.5577307200791305</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V49">
         <v>0.5639948157054135</v>
@@ -7420,16 +7450,16 @@
         <v>43921</v>
       </c>
       <c r="R50">
-        <v>0.5377117283672879</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S50">
-        <v>0.5202473277876889</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T50">
-        <v>0.5455881871447472</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U50">
-        <v>0.5561061205003087</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V50">
         <v>0.5645221577616581</v>
@@ -7533,25 +7563,25 @@
         <v>44012</v>
       </c>
       <c r="R51">
-        <v>0.5377022664239328</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S51">
-        <v>0.5202333474203812</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T51">
-        <v>0.5450430400268638</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U51">
-        <v>0.5554941239839795</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V51">
-        <v>0.5662039376373252</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W51">
-        <v>0.5804088423040777</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X51">
-        <v>0.5952331402543498</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y51">
         <v>0.5923719208076079</v>
@@ -7646,25 +7676,25 @@
         <v>44104</v>
       </c>
       <c r="R52">
-        <v>0.5376991926740736</v>
+        <v>0.6178545989638323</v>
       </c>
       <c r="S52">
-        <v>0.5202289754833684</v>
+        <v>0.5473174699944352</v>
       </c>
       <c r="T52">
-        <v>0.5448921977799999</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U52">
-        <v>0.5553224712343631</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V52">
-        <v>0.5664557585710209</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W52">
-        <v>0.5785137361133543</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X52">
-        <v>0.5875388759479933</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y52">
         <v>0.5921635512616348</v>
@@ -7759,19 +7789,19 @@
         <v>44196</v>
       </c>
       <c r="T53">
-        <v>0.544843179342028</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U53">
-        <v>0.5552654555290714</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V53">
-        <v>0.5665873118098071</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W53">
-        <v>0.5773918083128403</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X53">
-        <v>0.5830376389750327</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y53">
         <v>0.5925698485446134</v>
@@ -7866,19 +7896,19 @@
         <v>44286</v>
       </c>
       <c r="T54">
-        <v>0.5448286762748924</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U54">
-        <v>0.5552483119179632</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V54">
-        <v>0.5666193390735231</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W54">
-        <v>0.5771296896557584</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X54">
-        <v>0.5819824204821887</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y54">
         <v>0.5929756788467131</v>
@@ -7973,31 +8003,31 @@
         <v>44377</v>
       </c>
       <c r="T55">
-        <v>0.5448241473640095</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U55">
-        <v>0.5552428505696317</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V55">
-        <v>0.5666312492624046</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W55">
-        <v>0.577027862191363</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X55">
-        <v>0.5815738237463352</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y55">
-        <v>0.7051191129221102</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z55">
-        <v>0.6935829271408209</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA55">
-        <v>0.6909074213894455</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB55">
-        <v>0.6917643758788726</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC55">
         <v>0.3208668783516373</v>
@@ -8080,31 +8110,31 @@
         <v>44469</v>
       </c>
       <c r="T56">
-        <v>0.5448227766924101</v>
+        <v>0.7713113013799842</v>
       </c>
       <c r="U56">
-        <v>0.5552411686308616</v>
+        <v>0.8151983020565865</v>
       </c>
       <c r="V56">
-        <v>0.5666346892014176</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W56">
-        <v>0.576998686512222</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X56">
-        <v>0.5814567131233184</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y56">
-        <v>0.7259722410699202</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z56">
-        <v>0.7297356764283816</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA56">
-        <v>0.7302925783013771</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB56">
-        <v>0.7276687385283467</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC56">
         <v>0.3210953086939554</v>
@@ -8187,25 +8217,25 @@
         <v>44561</v>
       </c>
       <c r="V57">
-        <v>0.5666358384800969</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W57">
-        <v>0.5769887299525424</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X57">
-        <v>0.5814168026724831</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y57">
-        <v>0.7213968076784474</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z57">
-        <v>0.7223538575974726</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA57">
-        <v>0.722355911821677</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB57">
-        <v>0.7204506884645503</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC57">
         <v>0.3212121583454461</v>
@@ -8288,25 +8318,25 @@
         <v>44651</v>
       </c>
       <c r="V58">
-        <v>0.5666361908794398</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W58">
-        <v>0.5769856652752122</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X58">
-        <v>0.5814045245180548</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y58">
-        <v>0.7189718410834537</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z58">
-        <v>0.7183357346784771</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA58">
-        <v>0.718004947460972</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB58">
-        <v>0.7164891410725641</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC58">
         <v>0.3213289040714358</v>
@@ -8389,37 +8419,37 @@
         <v>44742</v>
       </c>
       <c r="V59">
-        <v>0.5666363044676379</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W59">
-        <v>0.5769846636170284</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X59">
-        <v>0.5814005152009492</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y59">
-        <v>0.7188653720122123</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z59">
-        <v>0.7181242757845959</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA59">
-        <v>0.7177675497972528</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB59">
-        <v>0.7162721366053887</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC59">
-        <v>0.6529833468746079</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD59">
-        <v>0.6657393685641638</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE59">
-        <v>0.6578281917221013</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF59">
-        <v>0.6271934745412224</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG59">
         <v>0.565387649938387</v>
@@ -8490,37 +8520,37 @@
         <v>44834</v>
       </c>
       <c r="V60">
-        <v>0.5666363400237209</v>
+        <v>0.7185938163272837</v>
       </c>
       <c r="W60">
-        <v>0.5769843475614326</v>
+        <v>0.7661325542161365</v>
       </c>
       <c r="X60">
-        <v>0.5813992510747694</v>
+        <v>0.7850413908864382</v>
       </c>
       <c r="Y60">
-        <v>0.7190284557915153</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z60">
-        <v>0.7183781491532431</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA60">
-        <v>0.7180395837608304</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB60">
-        <v>0.7165194947440002</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC60">
-        <v>0.7311570548637623</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD60">
-        <v>0.7270106815104631</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE60">
-        <v>0.7145400796873028</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF60">
-        <v>0.6383152965571581</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG60">
         <v>0.5659040305895076</v>
@@ -8591,28 +8621,28 @@
         <v>44926</v>
       </c>
       <c r="Y61">
-        <v>0.7190668565868102</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z61">
-        <v>0.7184410001846019</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA61">
-        <v>0.7181077894332965</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB61">
-        <v>0.7165815833538276</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC61">
-        <v>0.7249684190273153</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD61">
-        <v>0.7219575661424426</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE61">
-        <v>0.7114424489829182</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF61">
-        <v>0.63760009126303</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG61">
         <v>0.5661083054555434</v>
@@ -8683,28 +8713,28 @@
         <v>45016</v>
       </c>
       <c r="Y62">
-        <v>0.7190617066032733</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z62">
-        <v>0.7184342026006248</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA62">
-        <v>0.718100773188742</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB62">
-        <v>0.7165752263853495</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC62">
-        <v>0.717707143425698</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD62">
-        <v>0.7162471653020995</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE62">
-        <v>0.7072100675742921</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF62">
-        <v>0.637389980797599</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG62">
         <v>0.5663128372205222</v>
@@ -8775,40 +8805,40 @@
         <v>45107</v>
       </c>
       <c r="Y63">
-        <v>0.7190578510533461</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z63">
-        <v>0.7184283443360857</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA63">
-        <v>0.7180944981874205</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB63">
-        <v>0.7165695225723289</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC63">
-        <v>0.7164547588429951</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD63">
-        <v>0.715285703937004</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE63">
-        <v>0.706455328751925</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF63">
-        <v>0.6373810985845583</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG63">
-        <v>0.5455785622608329</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH63">
-        <v>0.5313729211371198</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI63">
-        <v>0.513532723422878</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ63">
-        <v>0.4538200343042281</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK63">
         <v>0.4227717190683649</v>
@@ -8867,40 +8897,40 @@
         <v>45199</v>
       </c>
       <c r="Y64">
-        <v>0.7190575215133579</v>
+        <v>0.6374576129581471</v>
       </c>
       <c r="Z64">
-        <v>0.7184277465647391</v>
+        <v>0.6345367160555659</v>
       </c>
       <c r="AA64">
-        <v>0.7180938335688147</v>
+        <v>0.6329650077197658</v>
       </c>
       <c r="AB64">
-        <v>0.7165689167634746</v>
+        <v>0.6255528669558384</v>
       </c>
       <c r="AC64">
-        <v>0.7166984929060538</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD64">
-        <v>0.7154830371627354</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE64">
-        <v>0.7065503535634486</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF64">
-        <v>0.637383109827265</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG64">
-        <v>0.5414597810972493</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH64">
-        <v>0.5562527733740431</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI64">
-        <v>0.5324448580453739</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ64">
-        <v>0.4687486084061045</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK64">
         <v>0.4227483540697676</v>
@@ -8959,28 +8989,28 @@
         <v>45291</v>
       </c>
       <c r="AC65">
-        <v>0.7168489069836395</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD65">
-        <v>0.7156002395552937</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE65">
-        <v>0.7066187302212102</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF65">
-        <v>0.6373834035466607</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG65">
-        <v>0.540783364039983</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH65">
-        <v>0.559873705932431</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI65">
-        <v>0.5364757554579683</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ65">
-        <v>0.4709317229228321</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK65">
         <v>0.379900233589936</v>
@@ -9039,28 +9069,28 @@
         <v>45382</v>
       </c>
       <c r="AC66">
-        <v>0.7168662737330975</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD66">
-        <v>0.7156130526104798</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE66">
-        <v>0.706628116905143</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF66">
-        <v>0.6373834025428466</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG66">
-        <v>0.5406771474830102</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH66">
-        <v>0.560311483594657</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI66">
-        <v>0.5371770109519639</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ66">
-        <v>0.4712503159604675</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK66">
         <v>0.3812601305627368</v>
@@ -9119,40 +9149,40 @@
         <v>45473</v>
       </c>
       <c r="AC67">
-        <v>0.7168592032707914</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD67">
-        <v>0.7156073846309035</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE67">
-        <v>0.7066259530749028</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF67">
-        <v>0.637383398557781</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG67">
-        <v>0.5406606708266285</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH67">
-        <v>0.5603568725715128</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI67">
-        <v>0.5373072519643562</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ67">
-        <v>0.4712968052810405</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK67">
-        <v>0.5251360674369788</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL67">
-        <v>0.549477353466623</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM67">
-        <v>0.6064845945658025</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN67">
-        <v>0.4828677335628926</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO67">
         <v>1.033334771491255</v>
@@ -9199,40 +9229,40 @@
         <v>45565</v>
       </c>
       <c r="AC68">
-        <v>0.7168562474817939</v>
+        <v>0.4566514387592278</v>
       </c>
       <c r="AD68">
-        <v>0.7156051124468924</v>
+        <v>0.44990971690776</v>
       </c>
       <c r="AE68">
-        <v>0.7066248827138775</v>
+        <v>0.4058476413602478</v>
       </c>
       <c r="AF68">
-        <v>0.6373833982226454</v>
+        <v>0.07668996647780491</v>
       </c>
       <c r="AG68">
-        <v>0.540658123707054</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH68">
-        <v>0.560360811481009</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI68">
-        <v>0.5373309137107601</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ68">
-        <v>0.4713035890035093</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK68">
-        <v>0.5462372164700643</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL68">
-        <v>0.5742081514664457</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM68">
-        <v>0.6161556561152235</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN68">
-        <v>0.5084091828181839</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO68">
         <v>0.9051321049412735</v>
@@ -9279,28 +9309,28 @@
         <v>45657</v>
       </c>
       <c r="AG69">
-        <v>0.5406577303356649</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH69">
-        <v>0.5603610623029985</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI69">
-        <v>0.5373352440941201</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ69">
-        <v>0.4713045788841876</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK69">
-        <v>0.5544656401998117</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL69">
-        <v>0.5851635910188951</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM69">
-        <v>0.6209203173300034</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN69">
-        <v>0.5191753993704133</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO69">
         <v>0.7816402422690345</v>
@@ -9347,28 +9377,28 @@
         <v>45747</v>
       </c>
       <c r="AG70">
-        <v>0.5406576696013498</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH70">
-        <v>0.5603610653760713</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI70">
-        <v>0.5373360346707097</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ70">
-        <v>0.4713047233275595</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK70">
-        <v>0.5564236214879722</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL70">
-        <v>0.5878690801450143</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM70">
-        <v>0.6221044916514983</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN70">
-        <v>0.5209906473480685</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO70">
         <v>0.7822113523727126</v>
@@ -9415,40 +9445,40 @@
         <v>45838</v>
       </c>
       <c r="AG71">
-        <v>0.5406576602250698</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH71">
-        <v>0.5603610629220809</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI71">
-        <v>0.5373361791200465</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ71">
-        <v>0.4713047444047338</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK71">
-        <v>0.5570041305627913</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL71">
-        <v>0.5887495320309113</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM71">
-        <v>0.6225088106322079</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN71">
-        <v>0.5214972361556129</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO71">
-        <v>0.4401409674393709</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP71">
-        <v>0.423123739728878</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ71">
-        <v>0.4282506763823117</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR71">
-        <v>0.1323981416292124</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS71">
         <v>0.1991269897618366</v>
@@ -9483,40 +9513,40 @@
         <v>45930</v>
       </c>
       <c r="AG72">
-        <v>0.540657658777575</v>
+        <v>0.5488696681700105</v>
       </c>
       <c r="AH72">
-        <v>0.5603610623801794</v>
+        <v>0.6463113775018655</v>
       </c>
       <c r="AI72">
-        <v>0.5373362055057748</v>
+        <v>0.5405987680679587</v>
       </c>
       <c r="AJ72">
-        <v>0.4713047474803148</v>
+        <v>0.2220039936166884</v>
       </c>
       <c r="AK72">
-        <v>0.5571590335545917</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL72">
-        <v>0.5889984059809437</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM72">
-        <v>0.6226262345316161</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN72">
-        <v>0.5216016924561634</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO72">
-        <v>0.4098040190116147</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP72">
-        <v>0.383426006203817</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ72">
-        <v>0.4030946197612124</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR72">
-        <v>0.1646134155832848</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS72">
         <v>0.2623745466969467</v>
@@ -9551,28 +9581,28 @@
         <v>46022</v>
       </c>
       <c r="AK73">
-        <v>0.5572024417289252</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL73">
-        <v>0.5890738213634863</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM73">
-        <v>0.6226631518292187</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN73">
-        <v>0.5216273375648952</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO73">
-        <v>0.3874554247116007</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP73">
-        <v>0.361771369730591</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ73">
-        <v>0.394118829171132</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR73">
-        <v>0.18524485659104</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS73">
         <v>0.3428813742886376</v>
@@ -9607,28 +9637,28 @@
         <v>46112</v>
       </c>
       <c r="AK74">
-        <v>0.5572143282206879</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL74">
-        <v>0.5890958891398977</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM74">
-        <v>0.6226743068244912</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN74">
-        <v>0.5216330154484716</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO74">
-        <v>0.3837281195185614</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP74">
-        <v>0.3574508066235254</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ74">
-        <v>0.3921245392893833</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR74">
-        <v>0.1905348862634995</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS74">
         <v>0.3417625854768005</v>
@@ -9663,40 +9693,40 @@
         <v>46203</v>
       </c>
       <c r="AK75">
-        <v>0.5572176185157496</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL75">
-        <v>0.5891024599960041</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM75">
-        <v>0.6226777443600073</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN75">
-        <v>0.5216343507171429</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO75">
-        <v>0.3821130607885287</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP75">
-        <v>0.3557973807028501</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ75">
-        <v>0.3915026902630535</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR75">
-        <v>0.1929626774048818</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS75">
-        <v>0.09523017641380505</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT75">
-        <v>0.09478569687886393</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU75">
-        <v>0.1287636306818425</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV75">
-        <v>0.1019123968419991</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW75">
         <v>0.2817932142556572</v>
@@ -9719,40 +9749,40 @@
         <v>46295</v>
       </c>
       <c r="AK76">
-        <v>0.5572185246807418</v>
+        <v>0.7050075432870883</v>
       </c>
       <c r="AL76">
-        <v>0.5891043995390788</v>
+        <v>0.8587412280225181</v>
       </c>
       <c r="AM76">
-        <v>0.6226787933550471</v>
+        <v>1.015723911283067</v>
       </c>
       <c r="AN76">
-        <v>0.5216346537719909</v>
+        <v>0.5328027202711724</v>
       </c>
       <c r="AO76">
-        <v>0.3817555030001082</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP76">
-        <v>0.3553931855675422</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ76">
-        <v>0.391351251749228</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR76">
-        <v>0.1937150072545304</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS76">
-        <v>0.09692216316865673</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT76">
-        <v>0.09402571203260346</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU76">
-        <v>0.1289854143988236</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV76">
-        <v>0.1016639383736171</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW76">
         <v>0.3121257356490901</v>
@@ -9775,28 +9805,28 @@
         <v>46387</v>
       </c>
       <c r="AO77">
-        <v>0.3816309576697509</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP77">
-        <v>0.3552599632780444</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ77">
-        <v>0.3913071840589675</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR77">
-        <v>0.1940164283578897</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS77">
-        <v>0.08313344033046377</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT77">
-        <v>0.08024385092079667</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU77">
-        <v>0.1044725722553859</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV77">
-        <v>0.07132023275963027</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW77">
         <v>0.3332836563751727</v>
@@ -9819,28 +9849,28 @@
         <v>46477</v>
       </c>
       <c r="AO78">
-        <v>0.3815993551479101</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP78">
-        <v>0.3552241648872401</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ78">
-        <v>0.3912959185443233</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR78">
-        <v>0.1941181083610441</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS78">
-        <v>0.08332612237782525</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT78">
-        <v>0.08014973469007496</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU78">
-        <v>0.1045015060664315</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV78">
-        <v>0.07112600606709764</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW78">
         <v>0.3337454255914167</v>
@@ -9863,40 +9893,40 @@
         <v>46568</v>
       </c>
       <c r="AO79">
-        <v>0.3815893930866359</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP79">
-        <v>0.3552131273523486</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ79">
-        <v>0.3912927560297575</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR79">
-        <v>0.194156533868595</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS79">
-        <v>0.08255421208711736</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT79">
-        <v>0.07929642391887824</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU79">
-        <v>0.1030511732486628</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV79">
-        <v>0.06901991718867434</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW79">
-        <v>0.1213878857341459</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX79">
-        <v>0.08612675401285461</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY79">
-        <v>0.08559836345893969</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ79">
-        <v>0.1860443245947445</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA79">
         <v>0.605709523522961</v>
@@ -9907,40 +9937,40 @@
         <v>46660</v>
       </c>
       <c r="AO80">
-        <v>0.3815866927659092</v>
+        <v>0.3341862308644067</v>
       </c>
       <c r="AP80">
-        <v>0.3552100282957382</v>
+        <v>0.2075849893335687</v>
       </c>
       <c r="AQ80">
-        <v>0.3912919265777365</v>
+        <v>0.3826810133150929</v>
       </c>
       <c r="AR80">
-        <v>0.1941699960394563</v>
+        <v>-0.527416572551914</v>
       </c>
       <c r="AS80">
-        <v>0.08257047299571642</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT80">
-        <v>0.07928768393415792</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU80">
-        <v>0.1030538206605628</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV80">
-        <v>0.06899415904730528</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW80">
-        <v>0.1132217155851031</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX80">
-        <v>0.08422870947730488</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY80">
-        <v>0.0827643559280878</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ80">
-        <v>0.1618475100643087</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA80">
         <v>0.6297219506583787</v>
@@ -9951,28 +9981,28 @@
         <v>46752</v>
       </c>
       <c r="AS81">
-        <v>0.08252722151382555</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT81">
-        <v>0.07923484082427794</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU81">
-        <v>0.1029680093106547</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV81">
-        <v>0.06884790850717135</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW81">
-        <v>0.09738150340351992</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX81">
-        <v>0.07104645159853472</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY81">
-        <v>0.06765811452014722</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ81">
-        <v>0.1150567307023475</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA81">
         <v>0.688907477092755</v>
@@ -9983,28 +10013,28 @@
         <v>46843</v>
       </c>
       <c r="AS82">
-        <v>0.08252843801259697</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT82">
-        <v>0.07923411937452331</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU82">
-        <v>0.1029682212981856</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV82">
-        <v>0.06884526859274784</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW82">
-        <v>0.09617284620716506</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX82">
-        <v>0.07039989653475497</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY82">
-        <v>0.0668502009818488</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ82">
-        <v>0.11071931544727</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA82">
         <v>0.6890597288883242</v>
@@ -10015,31 +10045,31 @@
         <v>46934</v>
       </c>
       <c r="AS83">
-        <v>0.08252601238326861</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT83">
-        <v>0.07923084633538288</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU83">
-        <v>0.1029631440914483</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV83">
-        <v>0.06883510773125348</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW83">
-        <v>0.0949681403021268</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX83">
-        <v>0.0693776277956378</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY83">
-        <v>0.0656538135032113</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ83">
-        <v>0.106580912411639</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA83">
-        <v>0.1926572091846671</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="84" spans="1:53">
@@ -10047,31 +10077,31 @@
         <v>47026</v>
       </c>
       <c r="AS84">
-        <v>0.08252609762601232</v>
+        <v>-0.1843269331972792</v>
       </c>
       <c r="AT84">
-        <v>0.07923079050252425</v>
+        <v>-0.1973133589982837</v>
       </c>
       <c r="AU84">
-        <v>0.1029631599088165</v>
+        <v>-0.0873644101196632</v>
       </c>
       <c r="AV84">
-        <v>0.06883486533222043</v>
+        <v>-0.2476439673034349</v>
       </c>
       <c r="AW84">
-        <v>0.09483326038585478</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX84">
-        <v>0.06928969752491428</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY84">
-        <v>0.06554483626001922</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ84">
-        <v>0.1060129947336498</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA84">
-        <v>0.1634322146850423</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="85" spans="1:53">
@@ -10079,19 +10109,19 @@
         <v>47118</v>
       </c>
       <c r="AW85">
-        <v>0.094739979370842</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX85">
-        <v>0.06920898002532046</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY85">
-        <v>0.06544832911151326</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ85">
-        <v>0.1056378838995605</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA85">
-        <v>0.1167069974641312</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="86" spans="1:53">
@@ -10099,19 +10129,19 @@
         <v>47208</v>
       </c>
       <c r="AW86">
-        <v>0.0947265167316808</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX86">
-        <v>0.06919924622208821</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY86">
-        <v>0.06543616042118486</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ86">
-        <v>0.1055717487867866</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA86">
-        <v>0.1113052809396471</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="87" spans="1:53">
@@ -10119,19 +10149,19 @@
         <v>47299</v>
       </c>
       <c r="AW87">
-        <v>0.09471917736546515</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX87">
-        <v>0.0691927663591371</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY87">
-        <v>0.0654282438332261</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ87">
-        <v>0.1055370251769951</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA87">
-        <v>0.1067510067757505</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="88" spans="1:53">
@@ -10139,19 +10169,19 @@
         <v>47391</v>
       </c>
       <c r="AW88">
-        <v>0.0947179097476003</v>
+        <v>0.1281137465774094</v>
       </c>
       <c r="AX88">
-        <v>0.06919178251509035</v>
+        <v>0.007682053153739344</v>
       </c>
       <c r="AY88">
-        <v>0.06542699661594611</v>
+        <v>-0.01085671717353166</v>
       </c>
       <c r="AZ88">
-        <v>0.1055297655091035</v>
+        <v>0.1697872170077176</v>
       </c>
       <c r="BA88">
-        <v>0.1059930343883705</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="89" spans="1:53">
@@ -10159,7 +10189,7 @@
         <v>47483</v>
       </c>
       <c r="BA89">
-        <v>0.1055354985232522</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="90" spans="1:53">
@@ -10167,7 +10197,7 @@
         <v>47573</v>
       </c>
       <c r="BA90">
-        <v>0.1054398312915992</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="91" spans="1:53">
@@ -10175,7 +10205,7 @@
         <v>47664</v>
       </c>
       <c r="BA91">
-        <v>0.1053927161830733</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
     <row r="92" spans="1:53">
@@ -10183,7 +10213,7 @@
         <v>47756</v>
       </c>
       <c r="BA92">
-        <v>0.1053812678519329</v>
+        <v>0.4743185562201461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>